<commit_message>
Config accepts costs invoice
</commit_message>
<xml_diff>
--- a/SmartOCR/Resources/config.xlsx
+++ b/SmartOCR/Resources/config.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maksim.Chuvashov\source\repos\SmartOCR\SmartOCR\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306FE321-28D5-4C37-B854-7E2407288380}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FBD709-D951-4FEB-B741-0AC05DCDCB3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{0089FDF6-97CB-48E9-8B61-38489BB510D9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" activeTab="2" xr2:uid="{0089FDF6-97CB-48E9-8B61-38489BB510D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Invoices" sheetId="2" r:id="rId1"/>
-    <sheet name="Settlement" sheetId="3" r:id="rId2"/>
+    <sheet name="invoice_sales" sheetId="2" r:id="rId1"/>
+    <sheet name="settlement" sheetId="3" r:id="rId2"/>
+    <sheet name="invoice_costs" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>String</t>
   </si>
@@ -163,6 +164,42 @@
   </si>
   <si>
     <t>(\d+\s*)+[,]*\d{2,3};1,3</t>
+  </si>
+  <si>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Invoice ([a-z]{6}):;Number</t>
+  </si>
+  <si>
+    <t>(\d+-\d+);</t>
+  </si>
+  <si>
+    <t>Invoice ([a-z]{4}):;Date</t>
+  </si>
+  <si>
+    <t>([a-z]{3,}\s*\d+,\s*\d{4});</t>
+  </si>
+  <si>
+    <t>[a-z]{7}:;Product</t>
+  </si>
+  <si>
+    <t>(.*oil.*);</t>
+  </si>
+  <si>
+    <t>[a-z]{5}:;Total</t>
+  </si>
+  <si>
+    <t>\$([\d,]+\.*\d{2});</t>
   </si>
 </sst>
 </file>
@@ -559,7 +596,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -786,7 +823,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +866,7 @@
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -843,7 +880,7 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -869,4 +906,92 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBFF1BA-6E15-43F9-8226-7B1CD7ABEE60}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Config data is stored in corresponding class instance
</commit_message>
<xml_diff>
--- a/SmartOCR/Resources/config.xlsx
+++ b/SmartOCR/Resources/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maksim.Chuvashov\source\repos\SmartOCR\SmartOCR\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FBD709-D951-4FEB-B741-0AC05DCDCB3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B2285D-B58F-4B96-B261-382EFB097580}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" activeTab="2" xr2:uid="{0089FDF6-97CB-48E9-8B61-38489BB510D9}"/>
   </bookViews>
@@ -193,13 +193,13 @@
     <t>[a-z]{7}:;Product</t>
   </si>
   <si>
-    <t>(.*oil.*);</t>
-  </si>
-  <si>
     <t>[a-z]{5}:;Total</t>
   </si>
   <si>
     <t>\$([\d,]+\.*\d{2});</t>
+  </si>
+  <si>
+    <t>(?:\s*Product[\s:]*)?(.*oil.*);</t>
   </si>
 </sst>
 </file>
@@ -910,10 +910,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBFF1BA-6E15-43F9-8226-7B1CD7ABEE60}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +972,7 @@
         <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -985,10 +986,10 @@
         <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Word document is closed after reading
</commit_message>
<xml_diff>
--- a/SmartOCR/Resources/config.xlsx
+++ b/SmartOCR/Resources/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maksim.Chuvashov\source\repos\SmartOCR\SmartOCR\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6919DF5-B93B-494F-AF08-501FDA6168C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD46DAF-45D8-49CB-9407-353DA30FC136}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{0089FDF6-97CB-48E9-8B61-38489BB510D9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>String</t>
   </si>
@@ -88,30 +88,15 @@
     <t>\d{2}\.\d{2}\.\d{4};1</t>
   </si>
   <si>
-    <t>\bUSD\b;1</t>
-  </si>
-  <si>
-    <t>((\d{1,3}\s)+\d{1,3},\d{2});1</t>
-  </si>
-  <si>
     <t>[\d,\s]*(\d{2}\.\d{2}\.\d{4});-1</t>
   </si>
   <si>
     <t>^[gods]{4,6};Goods</t>
   </si>
   <si>
-    <t>^(\d{1,3},\d{3});1</t>
-  </si>
-  <si>
-    <t>^(\d{1,3},\d{3});</t>
-  </si>
-  <si>
     <t>ON\s;2</t>
   </si>
   <si>
-    <t>([a-z]{3}\/[a-z]{3});</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -139,9 +124,6 @@
     <t>(.*OIL);</t>
   </si>
   <si>
-    <t>\b[net]{3}\b;1</t>
-  </si>
-  <si>
     <t>([a-z]{6}),.*;Weight</t>
   </si>
   <si>
@@ -193,10 +175,25 @@
     <t>(\d+\s*)+[,]*\d{2,3};1;1</t>
   </si>
   <si>
-    <t>(\d+\s*)+[,]*\d{2,3};</t>
-  </si>
-  <si>
     <t>\b[net]{3}\b;1;1</t>
+  </si>
+  <si>
+    <t>(\d+\s*)+[,]*\d{2,3};;1</t>
+  </si>
+  <si>
+    <t>\bUSD\b;1;1</t>
+  </si>
+  <si>
+    <t>((\d{1,3}\s)+\d{1,3},\d{2});1;1</t>
+  </si>
+  <si>
+    <t>([a-z]{3}\/[a-z]{3});;1</t>
+  </si>
+  <si>
+    <t>^(\d{1,3},\d{3});1;1</t>
+  </si>
+  <si>
+    <t>^(\d{1,3},\d{3});;1</t>
   </si>
 </sst>
 </file>
@@ -593,8 +590,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,25 +664,25 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -696,61 +693,61 @@
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -842,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -864,13 +861,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -878,13 +875,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,7 +889,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -926,16 +923,16 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -960,16 +957,16 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -977,16 +974,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Node can store no more than two duplicate lines
</commit_message>
<xml_diff>
--- a/SmartOCR/Resources/config.xlsx
+++ b/SmartOCR/Resources/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maksim.Chuvashov\source\repos\SmartOCR\SmartOCR\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD46DAF-45D8-49CB-9407-353DA30FC136}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD0942D-00BE-42A4-A050-99729CB04330}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{0089FDF6-97CB-48E9-8B61-38489BB510D9}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>^[gods]{4,6};Goods</t>
   </si>
   <si>
-    <t>ON\s;2</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -181,19 +178,22 @@
     <t>(\d+\s*)+[,]*\d{2,3};;1</t>
   </si>
   <si>
+    <t>((\d{1,3}\s)+\d{1,3},\d{2});1;1</t>
+  </si>
+  <si>
+    <t>([a-z]{3}\/[a-z]{3});;1</t>
+  </si>
+  <si>
+    <t>^(\d{1,3},\d{3});1;1</t>
+  </si>
+  <si>
+    <t>^(\d{1,3},\d{3});;1</t>
+  </si>
+  <si>
     <t>\bUSD\b;1;1</t>
   </si>
   <si>
-    <t>((\d{1,3}\s)+\d{1,3},\d{2});1;1</t>
-  </si>
-  <si>
-    <t>([a-z]{3}\/[a-z]{3});;1</t>
-  </si>
-  <si>
-    <t>^(\d{1,3},\d{3});1;1</t>
-  </si>
-  <si>
-    <t>^(\d{1,3},\d{3});;1</t>
+    <t>ON\s*;1</t>
   </si>
 </sst>
 </file>
@@ -590,8 +590,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +664,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -676,13 +676,13 @@
         <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -693,22 +693,22 @@
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -718,36 +718,36 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,13 +861,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -875,13 +875,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,16 +923,16 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,16 +957,16 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,16 +974,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed case when semicolon was part of RE pattern
</commit_message>
<xml_diff>
--- a/SmartOCR/Resources/config.xlsx
+++ b/SmartOCR/Resources/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maksim.Chuvashov\source\repos\SmartOCR\SmartOCR\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD0942D-00BE-42A4-A050-99729CB04330}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E22E4D-B387-4151-9450-888B996A98C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{0089FDF6-97CB-48E9-8B61-38489BB510D9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" activeTab="1" xr2:uid="{0089FDF6-97CB-48E9-8B61-38489BB510D9}"/>
   </bookViews>
   <sheets>
     <sheet name="invoice_sales" sheetId="2" r:id="rId1"/>
@@ -103,15 +103,6 @@
     <t>-\s(\w+\s\d{4});</t>
   </si>
   <si>
-    <t>\w{3}\s(\w{3}) #;CTM</t>
-  </si>
-  <si>
-    <t>#\s*:\s*(.*);</t>
-  </si>
-  <si>
-    <t>([\d,]*\d{3}\.\d{2});</t>
-  </si>
-  <si>
     <t>(\b[a-z]{6}\b);Amount</t>
   </si>
   <si>
@@ -194,6 +185,15 @@
   </si>
   <si>
     <t>ON\s*;1</t>
+  </si>
+  <si>
+    <t>[a-z]{3}\s([a-z]{3})\s*#;CTM</t>
+  </si>
+  <si>
+    <t>([\d,]*\d{1,3}\.\d{2});</t>
+  </si>
+  <si>
+    <t>#\s*[:;]\s*(.*);</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -664,7 +664,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -676,13 +676,13 @@
         <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -693,22 +693,22 @@
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -718,36 +718,36 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -816,8 +816,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,13 +861,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -875,13 +875,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,16 +923,16 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,16 +957,16 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,16 +974,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>